<commit_message>
Cache Miss Analysis for 4096 added
</commit_message>
<xml_diff>
--- a/CacheMissAnalysis.xlsx
+++ b/CacheMissAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\HPC\Project\Commandline Serial Codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97879DD-423B-4028-8161-3849239A1272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C284864-AEFB-4284-8FCE-7C55F0F081B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="504" yWindow="1068" windowWidth="11832" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -365,7 +365,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -374,6 +374,7 @@
     <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -409,7 +410,9 @@
       <c r="E2" s="2">
         <v>364663010</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2">
+        <v>2750655492</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -427,7 +430,9 @@
       <c r="E3" s="2">
         <v>245449501</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2">
+        <v>1714405802</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>